<commit_message>
numerous changes to simulation and optimization for efficiency & bug fixes
- cache results of optimization to avoid having to recreate the models
each time
- modify simulationRunHelper to make it possible to reuse old
"ItemModels"
- fix bug related to highlighting of runs, deleting runs, etc.
- avoid simulating models unless they are supposed to be plotted
- change book-keeping for handles to runs in optimization
</commit_message>
<xml_diff>
--- a/Sessions/ABC/ABCparameters.xlsx
+++ b/Sessions/ABC/ABCparameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Include</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>k2</t>
-  </si>
-  <si>
-    <t>k3</t>
   </si>
   <si>
     <t>log</t>
@@ -390,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +412,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -426,7 +423,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>0.1</v>
@@ -446,7 +443,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>0.1</v>
@@ -456,26 +453,6 @@
       </c>
       <c r="F3">
         <v>2.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>0.01</v>
-      </c>
-      <c r="E4">
-        <v>0.12</v>
-      </c>
-      <c r="F4">
-        <v>0.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>